<commit_message>
svm accuracy + importance
</commit_message>
<xml_diff>
--- a/feature_analysis/metabolite_f.xlsx
+++ b/feature_analysis/metabolite_f.xlsx
@@ -957,7 +957,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>153</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
         <v>55</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
         <v>57</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="B57" t="s">
         <v>58</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s">
         <v>59</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
         <v>60</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="B60" t="s">
         <v>61</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
         <v>62</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B62" t="s">
         <v>63</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B63" t="s">
         <v>64</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="B64" t="s">
         <v>65</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B65" t="s">
         <v>66</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="B66" t="s">
         <v>67</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
         <v>68</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
         <v>69</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
         <v>70</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="B70" t="s">
         <v>71</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B71" t="s">
         <v>72</v>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="B73" t="s">
         <v>74</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B74" t="s">
         <v>75</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="B75" t="s">
         <v>76</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B76" t="s">
         <v>77</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="B77" t="s">
         <v>78</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="B78" t="s">
         <v>79</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="B79" t="s">
         <v>80</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
         <v>81</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
         <v>82</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B82" t="s">
         <v>83</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
         <v>84</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
         <v>85</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
         <v>86</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="B86" t="s">
         <v>87</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="B87" t="s">
         <v>88</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B88" t="s">
         <v>89</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="B89" t="s">
         <v>90</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="B90" t="s">
         <v>91</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B91" t="s">
         <v>92</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B92" t="s">
         <v>93</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B93" t="s">
         <v>94</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B94" t="s">
         <v>95</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B95" t="s">
         <v>96</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B96" t="s">
         <v>97</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="B97" t="s">
         <v>98</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B98" t="s">
         <v>99</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="1">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="B99" t="s">
         <v>100</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="B100" t="s">
         <v>101</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="1">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
         <v>102</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="1">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B102" t="s">
         <v>103</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="1">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B103" t="s">
         <v>104</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="1">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B104" t="s">
         <v>105</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="1">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="B105" t="s">
         <v>106</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="1">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="B106" t="s">
         <v>107</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="B107" t="s">
         <v>108</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="1">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B108" t="s">
         <v>109</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="1">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="B109" t="s">
         <v>110</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="1">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B110" t="s">
         <v>111</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="1">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="B111" t="s">
         <v>112</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="1">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B112" t="s">
         <v>113</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="1">
-        <v>111</v>
+        <v>176</v>
       </c>
       <c r="B113" t="s">
         <v>114</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="1">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B114" t="s">
         <v>115</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="1">
-        <v>113</v>
+        <v>56</v>
       </c>
       <c r="B115" t="s">
         <v>116</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="1">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="B116" t="s">
         <v>117</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B117" t="s">
         <v>118</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="B118" t="s">
         <v>119</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="1">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="B119" t="s">
         <v>120</v>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="1">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="B120" t="s">
         <v>121</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="1">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="B121" t="s">
         <v>122</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="1">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B122" t="s">
         <v>123</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="1">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B123" t="s">
         <v>124</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="1">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B124" t="s">
         <v>125</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="1">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B125" t="s">
         <v>126</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="1">
-        <v>124</v>
+        <v>58</v>
       </c>
       <c r="B126" t="s">
         <v>127</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="1">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="B127" t="s">
         <v>128</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="1">
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="B128" t="s">
         <v>129</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="1">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="B129" t="s">
         <v>130</v>
@@ -2749,7 +2749,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="1">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B130" t="s">
         <v>131</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="1">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="B131" t="s">
         <v>132</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="1">
-        <v>130</v>
+        <v>77</v>
       </c>
       <c r="B132" t="s">
         <v>133</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="1">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
         <v>134</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="1">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="B134" t="s">
         <v>135</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="1">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="B135" t="s">
         <v>136</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="1">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="B136" t="s">
         <v>137</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="1">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="B137" t="s">
         <v>138</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="1">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="B138" t="s">
         <v>139</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="1">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B139" t="s">
         <v>140</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="1">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="B140" t="s">
         <v>141</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="1">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="B141" t="s">
         <v>142</v>
@@ -2917,7 +2917,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B142" t="s">
         <v>143</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="1">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="1">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="B144" t="s">
         <v>145</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="1">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B145" t="s">
         <v>146</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="1">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="B146" t="s">
         <v>147</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="1">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="B147" t="s">
         <v>148</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="1">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B148" t="s">
         <v>149</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="1">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="B149" t="s">
         <v>150</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="1">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="B150" t="s">
         <v>151</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="1">
-        <v>149</v>
+        <v>44</v>
       </c>
       <c r="B151" t="s">
         <v>152</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="1">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="B152" t="s">
         <v>153</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="1">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="B153" t="s">
         <v>154</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="1">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="B154" t="s">
         <v>155</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="1">
-        <v>153</v>
+        <v>18</v>
       </c>
       <c r="B155" t="s">
         <v>156</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="1">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="B156" t="s">
         <v>157</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="1">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="B157" t="s">
         <v>158</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="1">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="B158" t="s">
         <v>159</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="1">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B159" t="s">
         <v>160</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="1">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="B160" t="s">
         <v>161</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="1">
-        <v>159</v>
+        <v>99</v>
       </c>
       <c r="B161" t="s">
         <v>162</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="1">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="B162" t="s">
         <v>163</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="1">
-        <v>161</v>
+        <v>69</v>
       </c>
       <c r="B163" t="s">
         <v>164</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="1">
-        <v>162</v>
+        <v>39</v>
       </c>
       <c r="B164" t="s">
         <v>165</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="1">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B165" t="s">
         <v>166</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="1">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="B166" t="s">
         <v>167</v>
@@ -3267,7 +3267,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="1">
-        <v>165</v>
+        <v>116</v>
       </c>
       <c r="B167" t="s">
         <v>168</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="1">
-        <v>166</v>
+        <v>36</v>
       </c>
       <c r="B168" t="s">
         <v>169</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="1">
-        <v>167</v>
+        <v>38</v>
       </c>
       <c r="B169" t="s">
         <v>170</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="1">
-        <v>168</v>
+        <v>4</v>
       </c>
       <c r="B170" t="s">
         <v>171</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="1">
-        <v>169</v>
+        <v>13</v>
       </c>
       <c r="B171" t="s">
         <v>172</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="1">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="B172" t="s">
         <v>173</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="1">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="B173" t="s">
         <v>174</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="1">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="B174" t="s">
         <v>175</v>
@@ -3379,7 +3379,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="1">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B175" t="s">
         <v>176</v>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="1">
-        <v>174</v>
+        <v>117</v>
       </c>
       <c r="B176" t="s">
         <v>177</v>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="1">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="B177" t="s">
         <v>178</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="1">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="B178" t="s">
         <v>179</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="1">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="B179" t="s">
         <v>180</v>
@@ -3449,7 +3449,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="1">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="B180" t="s">
         <v>181</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="1">
-        <v>179</v>
+        <v>61</v>
       </c>
       <c r="B181" t="s">
         <v>182</v>
@@ -3477,7 +3477,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="1">
-        <v>180</v>
+        <v>17</v>
       </c>
       <c r="B182" t="s">
         <v>183</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="1">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B183" t="s">
         <v>184</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="1">
-        <v>182</v>
+        <v>12</v>
       </c>
       <c r="B184" t="s">
         <v>185</v>
@@ -3519,7 +3519,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="1">
-        <v>183</v>
+        <v>51</v>
       </c>
       <c r="B185" t="s">
         <v>186</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="1">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B186" t="s">
         <v>187</v>
@@ -3547,7 +3547,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="1">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="B187" t="s">
         <v>188</v>

</xml_diff>